<commit_message>
Value sent in ppm on UART
</commit_message>
<xml_diff>
--- a/Datasheet.xlsx
+++ b/Datasheet.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dragos\Workspace\Sleep_well\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dragos\00_Repositories\00_Sleep well\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12000" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12000" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Message format" sheetId="4" r:id="rId1"/>
     <sheet name="PPM CO2" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1584,8 +1585,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E98"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2442,4 +2443,1287 @@
   </headerFooter>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B201"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35:XFD35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="6">
+        <v>400</v>
+      </c>
+      <c r="B1">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="6">
+        <v>399</v>
+      </c>
+      <c r="B2">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="6">
+        <v>398</v>
+      </c>
+      <c r="B3">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="6">
+        <v>397</v>
+      </c>
+      <c r="B4">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="6">
+        <v>396</v>
+      </c>
+      <c r="B5">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="6">
+        <v>395</v>
+      </c>
+      <c r="B6">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="6">
+        <v>394</v>
+      </c>
+      <c r="B7">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="6">
+        <v>393</v>
+      </c>
+      <c r="B8">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="6">
+        <v>392</v>
+      </c>
+      <c r="B9">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="6">
+        <v>391</v>
+      </c>
+      <c r="B10">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="6">
+        <v>390</v>
+      </c>
+      <c r="B11">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="6">
+        <v>389</v>
+      </c>
+      <c r="B12">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="6">
+        <v>388</v>
+      </c>
+      <c r="B13">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="6">
+        <v>387</v>
+      </c>
+      <c r="B14">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="6">
+        <v>386</v>
+      </c>
+      <c r="B15">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="6">
+        <v>385</v>
+      </c>
+      <c r="B16">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="6">
+        <v>384</v>
+      </c>
+      <c r="B17">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="6">
+        <v>383</v>
+      </c>
+      <c r="B18">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="6">
+        <v>382</v>
+      </c>
+      <c r="B19">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="6">
+        <v>381</v>
+      </c>
+      <c r="B20">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="6">
+        <v>380</v>
+      </c>
+      <c r="B21">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="6">
+        <v>379</v>
+      </c>
+      <c r="B22">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="6">
+        <v>378</v>
+      </c>
+      <c r="B23">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="6">
+        <v>377</v>
+      </c>
+      <c r="B24">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="6">
+        <v>376</v>
+      </c>
+      <c r="B25">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="6">
+        <v>375</v>
+      </c>
+      <c r="B26">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="6">
+        <v>374</v>
+      </c>
+      <c r="B27">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="6">
+        <v>373</v>
+      </c>
+      <c r="B28">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="6">
+        <v>372</v>
+      </c>
+      <c r="B29">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="6">
+        <v>371</v>
+      </c>
+      <c r="B30">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="6">
+        <v>370</v>
+      </c>
+      <c r="B31">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="6">
+        <v>369</v>
+      </c>
+      <c r="B32">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="6">
+        <v>368</v>
+      </c>
+      <c r="B33">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="6">
+        <v>367</v>
+      </c>
+      <c r="B34">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="6">
+        <v>366</v>
+      </c>
+      <c r="B35">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="6">
+        <v>365</v>
+      </c>
+      <c r="B36">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="6">
+        <v>364</v>
+      </c>
+      <c r="B37">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="6">
+        <v>363</v>
+      </c>
+      <c r="B38">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="6">
+        <v>362</v>
+      </c>
+      <c r="B39">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="6">
+        <v>361</v>
+      </c>
+      <c r="B40">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="6">
+        <v>360</v>
+      </c>
+      <c r="B41">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="6">
+        <v>359</v>
+      </c>
+      <c r="B42">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="6">
+        <v>358</v>
+      </c>
+      <c r="B43">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="6">
+        <v>357</v>
+      </c>
+      <c r="B44">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="6">
+        <v>356</v>
+      </c>
+      <c r="B45">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="6">
+        <v>355</v>
+      </c>
+      <c r="B46">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="6">
+        <v>354</v>
+      </c>
+      <c r="B47">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="6">
+        <v>353</v>
+      </c>
+      <c r="B48">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="6">
+        <v>352</v>
+      </c>
+      <c r="B49">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="6">
+        <v>351</v>
+      </c>
+      <c r="B50">
+        <v>852</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="6">
+        <v>350</v>
+      </c>
+      <c r="B51">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="6">
+        <v>349</v>
+      </c>
+      <c r="B52">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="6">
+        <v>348</v>
+      </c>
+      <c r="B53">
+        <v>891</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="6">
+        <v>347</v>
+      </c>
+      <c r="B54">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="6">
+        <v>346</v>
+      </c>
+      <c r="B55">
+        <v>915</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="6">
+        <v>345</v>
+      </c>
+      <c r="B56">
+        <v>930</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="6">
+        <v>344</v>
+      </c>
+      <c r="B57">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="6">
+        <v>343</v>
+      </c>
+      <c r="B58">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="6">
+        <v>342</v>
+      </c>
+      <c r="B59">
+        <v>975</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="6">
+        <v>341</v>
+      </c>
+      <c r="B60">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="6">
+        <v>340</v>
+      </c>
+      <c r="B61">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="6">
+        <v>339</v>
+      </c>
+      <c r="B62">
+        <v>1017</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" s="6">
+        <v>338</v>
+      </c>
+      <c r="B63">
+        <v>1034</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" s="6">
+        <v>337</v>
+      </c>
+      <c r="B64">
+        <v>1051</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="6">
+        <v>336</v>
+      </c>
+      <c r="B65">
+        <v>1068</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="6">
+        <v>335</v>
+      </c>
+      <c r="B66">
+        <v>1085</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" s="6">
+        <v>334</v>
+      </c>
+      <c r="B67">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" s="6">
+        <v>333</v>
+      </c>
+      <c r="B68">
+        <v>1119</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" s="6">
+        <v>332</v>
+      </c>
+      <c r="B69">
+        <v>1138</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" s="6">
+        <v>331</v>
+      </c>
+      <c r="B70">
+        <v>1157</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" s="6">
+        <v>330</v>
+      </c>
+      <c r="B71">
+        <v>1176</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" s="6">
+        <v>329</v>
+      </c>
+      <c r="B72">
+        <v>1195</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" s="6">
+        <v>328</v>
+      </c>
+      <c r="B73">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" s="6">
+        <v>327</v>
+      </c>
+      <c r="B74">
+        <v>1220</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" s="6">
+        <v>326</v>
+      </c>
+      <c r="B75">
+        <v>1240</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" s="6">
+        <v>325</v>
+      </c>
+      <c r="B76">
+        <v>1260</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" s="6">
+        <v>324</v>
+      </c>
+      <c r="B77">
+        <v>1280</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" s="6">
+        <v>323</v>
+      </c>
+      <c r="B78">
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" s="6">
+        <v>322</v>
+      </c>
+      <c r="B79">
+        <v>1320</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" s="6">
+        <v>321</v>
+      </c>
+      <c r="B80">
+        <v>1340</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" s="6">
+        <v>320</v>
+      </c>
+      <c r="B81">
+        <v>1360</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" s="6">
+        <v>319</v>
+      </c>
+      <c r="B82">
+        <v>1380</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" s="6">
+        <v>318</v>
+      </c>
+      <c r="B83">
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" s="6">
+        <v>317</v>
+      </c>
+      <c r="B84">
+        <v>1420</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" s="6">
+        <v>316</v>
+      </c>
+      <c r="B85">
+        <v>1440</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" s="6">
+        <v>315</v>
+      </c>
+      <c r="B86">
+        <v>1460</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" s="6">
+        <v>314</v>
+      </c>
+      <c r="B87">
+        <v>1480</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" s="6">
+        <v>313</v>
+      </c>
+      <c r="B88">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" s="6">
+        <v>312</v>
+      </c>
+      <c r="B89">
+        <v>1525</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" s="6">
+        <v>311</v>
+      </c>
+      <c r="B90">
+        <v>1550</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" s="6">
+        <v>310</v>
+      </c>
+      <c r="B91">
+        <v>1575</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" s="6">
+        <v>309</v>
+      </c>
+      <c r="B92">
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" s="6">
+        <v>308</v>
+      </c>
+      <c r="B93">
+        <v>1625</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" s="6">
+        <v>307</v>
+      </c>
+      <c r="B94">
+        <v>1650</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95" s="6">
+        <v>306</v>
+      </c>
+      <c r="B95">
+        <v>1675</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96" s="6">
+        <v>305</v>
+      </c>
+      <c r="B96">
+        <v>1700</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" s="6">
+        <v>304</v>
+      </c>
+      <c r="B97">
+        <v>1733</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" s="6">
+        <v>303</v>
+      </c>
+      <c r="B98">
+        <v>1766</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" s="6">
+        <v>302</v>
+      </c>
+      <c r="B99">
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" s="6">
+        <v>301</v>
+      </c>
+      <c r="B100">
+        <v>1825</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" s="6">
+        <v>300</v>
+      </c>
+      <c r="B101">
+        <v>1850</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102" s="6">
+        <v>299</v>
+      </c>
+      <c r="B102">
+        <v>1875</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103" s="6">
+        <v>298</v>
+      </c>
+      <c r="B103">
+        <v>1900</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104" s="6">
+        <v>297</v>
+      </c>
+      <c r="B104">
+        <v>1933</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105" s="6">
+        <v>296</v>
+      </c>
+      <c r="B105">
+        <v>1966</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" s="6">
+        <v>295</v>
+      </c>
+      <c r="B106">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" s="6">
+        <v>294</v>
+      </c>
+      <c r="B107">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108" s="6">
+        <v>293</v>
+      </c>
+      <c r="B108">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109" s="6">
+        <v>292</v>
+      </c>
+      <c r="B109">
+        <v>2075</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110" s="6">
+        <v>291</v>
+      </c>
+      <c r="B110">
+        <v>2100</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111" s="6">
+        <v>290</v>
+      </c>
+      <c r="B111">
+        <v>2133</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112" s="6">
+        <v>289</v>
+      </c>
+      <c r="B112">
+        <v>2166</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113" s="6">
+        <v>288</v>
+      </c>
+      <c r="B113">
+        <v>2200</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114" s="6">
+        <v>287</v>
+      </c>
+      <c r="B114">
+        <v>2234</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A115" s="6">
+        <v>286</v>
+      </c>
+      <c r="B115">
+        <v>2268</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A116" s="6">
+        <v>285</v>
+      </c>
+      <c r="B116">
+        <v>2300</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A117" s="6">
+        <v>284</v>
+      </c>
+      <c r="B117">
+        <v>2350</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A118" s="6">
+        <v>283</v>
+      </c>
+      <c r="B118">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A119" s="6">
+        <v>282</v>
+      </c>
+      <c r="B119">
+        <v>2433</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A120" s="6">
+        <v>281</v>
+      </c>
+      <c r="B120">
+        <v>2466</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A121" s="6">
+        <v>280</v>
+      </c>
+      <c r="B121">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A122" s="6">
+        <v>279</v>
+      </c>
+      <c r="B122">
+        <v>2533</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A123" s="6">
+        <v>278</v>
+      </c>
+      <c r="B123">
+        <v>2566</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A124" s="6">
+        <v>277</v>
+      </c>
+      <c r="B124">
+        <v>2600</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A125" s="6">
+        <v>276</v>
+      </c>
+      <c r="B125">
+        <v>2650</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A126" s="6">
+        <v>275</v>
+      </c>
+      <c r="B126">
+        <v>2700</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A127" s="6">
+        <v>274</v>
+      </c>
+      <c r="B127">
+        <v>2750</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A128" s="6">
+        <v>273</v>
+      </c>
+      <c r="B128">
+        <v>2800</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A129" s="6">
+        <v>272</v>
+      </c>
+      <c r="B129">
+        <v>2833</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A130" s="6">
+        <v>271</v>
+      </c>
+      <c r="B130">
+        <v>2866</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A131" s="6">
+        <v>270</v>
+      </c>
+      <c r="B131">
+        <v>2900</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A132" s="6">
+        <v>269</v>
+      </c>
+      <c r="B132">
+        <v>2950</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A133" s="6">
+        <v>268</v>
+      </c>
+      <c r="B133">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A134" s="6"/>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A135" s="6"/>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A136" s="6"/>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A137" s="6"/>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A138" s="6"/>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A139" s="6"/>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A140" s="6"/>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A141" s="6"/>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A142" s="6"/>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A143" s="6"/>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A144" s="6"/>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A145" s="6"/>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A146" s="6"/>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A147" s="6"/>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A148" s="6"/>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A149" s="6"/>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A150" s="6"/>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A151" s="6"/>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A152" s="6"/>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A153" s="6"/>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A154" s="6"/>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A155" s="6"/>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A156" s="6"/>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A157" s="6"/>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A158" s="6"/>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A159" s="6"/>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A160" s="6"/>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A161" s="6"/>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A162" s="6"/>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A163" s="6"/>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A164" s="6"/>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A165" s="6"/>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A166" s="6"/>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A167" s="6"/>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A168" s="6"/>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A169" s="6"/>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A170" s="6"/>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A171" s="6"/>
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A172" s="6"/>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A173" s="6"/>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A174" s="6"/>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A175" s="6"/>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A176" s="6"/>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A177" s="6"/>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A178" s="6"/>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A179" s="6"/>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A180" s="6"/>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A181" s="6"/>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A182" s="6"/>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A183" s="6"/>
+    </row>
+    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A184" s="6"/>
+    </row>
+    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A185" s="6"/>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A186" s="6"/>
+    </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A187" s="6"/>
+    </row>
+    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A188" s="6"/>
+    </row>
+    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A189" s="6"/>
+    </row>
+    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A190" s="6"/>
+    </row>
+    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A191" s="6"/>
+    </row>
+    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A192" s="6"/>
+    </row>
+    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A193" s="6"/>
+    </row>
+    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A194" s="6"/>
+    </row>
+    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A195" s="6"/>
+    </row>
+    <row r="196" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A196" s="6"/>
+    </row>
+    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A197" s="6"/>
+    </row>
+    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A198" s="6"/>
+    </row>
+    <row r="199" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A199" s="6"/>
+    </row>
+    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A200" s="6"/>
+    </row>
+    <row r="201" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A201" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>